<commit_message>
Log and supplemental Framework specification
</commit_message>
<xml_diff>
--- a/doc/log/201608040123-张宏权.xlsx
+++ b/doc/log/201608040123-张宏权.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9420"/>
+    <workbookView windowWidth="18215" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34">
   <si>
     <t>时间</t>
   </si>
@@ -82,6 +82,42 @@
   </si>
   <si>
     <t>前后端掌握技术少</t>
+  </si>
+  <si>
+    <t>复习视频内容</t>
+  </si>
+  <si>
+    <t>数据库使用</t>
+  </si>
+  <si>
+    <t>不操作遗忘</t>
+  </si>
+  <si>
+    <t>数据库安装配置</t>
+  </si>
+  <si>
+    <t>复习MySQL</t>
+  </si>
+  <si>
+    <t>mybatis没操作过</t>
+  </si>
+  <si>
+    <t>看视频学习springboot</t>
+  </si>
+  <si>
+    <t>准备学习mybatis</t>
+  </si>
+  <si>
+    <t>配置出错</t>
+  </si>
+  <si>
+    <t>补充架构说明书</t>
+  </si>
+  <si>
+    <t xml:space="preserve">整合Mybatis </t>
+  </si>
+  <si>
+    <t>逻辑结构不清晰</t>
   </si>
 </sst>
 </file>
@@ -89,9 +125,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -103,20 +139,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +147,57 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -140,29 +213,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -193,31 +254,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -238,14 +282,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -256,187 +292,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,11 +568,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -544,8 +586,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -595,17 +637,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -617,145 +653,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1135,7 +1171,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19:O20"/>
+      <selection activeCell="D27" sqref="D27:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1477,18 +1513,26 @@
       <c r="O16" s="7"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1">
+        <v>181117</v>
+      </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="2"/>
+      <c r="L17" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="4"/>
@@ -1511,18 +1555,26 @@
       <c r="O18" s="7"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1">
+        <v>181118</v>
+      </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="2"/>
+      <c r="L19" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="4"/>
@@ -1545,18 +1597,26 @@
       <c r="O20" s="7"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1">
+        <v>181119</v>
+      </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="2"/>
+      <c r="L21" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="4"/>
@@ -1579,18 +1639,26 @@
       <c r="O22" s="7"/>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="1"/>
+      <c r="A23" s="1">
+        <v>181120</v>
+      </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="H23" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
-      <c r="L23" s="2"/>
+      <c r="L23" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="4"/>

</xml_diff>

<commit_message>
Enterprise information module specification and daily
</commit_message>
<xml_diff>
--- a/doc/log/201608040123-张宏权.xlsx
+++ b/doc/log/201608040123-张宏权.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48">
   <si>
     <t>时间</t>
   </si>
@@ -142,6 +142,24 @@
   </si>
   <si>
     <t>学习进程缓慢</t>
+  </si>
+  <si>
+    <t>登录模块简单实现</t>
+  </si>
+  <si>
+    <t>注册模块，详细说明书</t>
+  </si>
+  <si>
+    <t>定义变量统一问题</t>
+  </si>
+  <si>
+    <t>详细设计说明书</t>
+  </si>
+  <si>
+    <t>注册模块完成</t>
+  </si>
+  <si>
+    <t>前端框架应用</t>
   </si>
 </sst>
 </file>
@@ -149,10 +167,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -164,36 +182,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -206,9 +195,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -230,8 +255,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -239,7 +265,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -269,22 +295,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -293,7 +303,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -306,6 +316,14 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -316,6 +334,138 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -328,25 +478,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -358,145 +502,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -589,6 +607,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -598,17 +625,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -628,24 +658,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -661,11 +673,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -677,10 +695,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -689,142 +707,139 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1197,7 +1212,7 @@
   <sheetPr/>
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="L33" sqref="L33:O34"/>
     </sheetView>
   </sheetViews>
@@ -1221,12 +1236,12 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="5"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="4"/>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="1"/>
@@ -1240,10 +1255,10 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="8"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="7"/>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="1">
@@ -1263,12 +1278,12 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="5"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="1"/>
@@ -1282,10 +1297,10 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="8"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="7"/>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="1">
@@ -1305,12 +1320,12 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="5"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1"/>
@@ -1324,10 +1339,10 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="8"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="7"/>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="1">
@@ -1347,12 +1362,12 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="5"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="4"/>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="1"/>
@@ -1366,10 +1381,10 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="8"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="7"/>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="1">
@@ -1389,12 +1404,12 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="5"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="1"/>
@@ -1408,10 +1423,10 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="8"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="7"/>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="1">
@@ -1431,12 +1446,12 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="3" t="s">
+      <c r="L11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="5"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="4"/>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="1"/>
@@ -1450,10 +1465,10 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="8"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="7"/>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="1">
@@ -1473,12 +1488,12 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="3" t="s">
+      <c r="L13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="5"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="4"/>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="1"/>
@@ -1492,10 +1507,10 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="8"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="7"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1">
@@ -1515,12 +1530,12 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="3" t="s">
+      <c r="L15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="5"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="4"/>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="1"/>
@@ -1534,10 +1549,10 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="8"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="7"/>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="1">
@@ -1557,12 +1572,12 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="3" t="s">
+      <c r="L17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="5"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="4"/>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="1"/>
@@ -1576,10 +1591,10 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="8"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="7"/>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="1">
@@ -1599,12 +1614,12 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="3" t="s">
+      <c r="L19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="5"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="4"/>
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="1"/>
@@ -1618,10 +1633,10 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="8"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="7"/>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="1">
@@ -1641,12 +1656,12 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="3" t="s">
+      <c r="L21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="5"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="4"/>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="1"/>
@@ -1660,10 +1675,10 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="8"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="7"/>
     </row>
     <row r="23" spans="1:15">
       <c r="A23" s="1">
@@ -1683,12 +1698,12 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
-      <c r="L23" s="3" t="s">
+      <c r="L23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="5"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="4"/>
     </row>
     <row r="24" spans="1:15">
       <c r="A24" s="1"/>
@@ -1702,10 +1717,10 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="8"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="7"/>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" s="1">
@@ -1725,12 +1740,12 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
-      <c r="L25" s="3" t="s">
+      <c r="L25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="5"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="4"/>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="1"/>
@@ -1744,10 +1759,10 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="8"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="7"/>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="1">
@@ -1767,12 +1782,12 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
-      <c r="L27" s="3" t="s">
+      <c r="L27" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="5"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="4"/>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="1"/>
@@ -1786,10 +1801,10 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="8"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="7"/>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="1">
@@ -1797,41 +1812,41 @@
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
       <c r="H29" s="1" t="s">
         <v>40</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
-      <c r="L29" s="3" t="s">
+      <c r="L29" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="5"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="4"/>
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="8"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="7"/>
     </row>
     <row r="31" spans="1:15">
       <c r="A31" s="1">
@@ -1839,35 +1854,41 @@
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="5"/>
+      <c r="L31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="4"/>
     </row>
     <row r="32" spans="1:15">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="8"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="7"/>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="1">
@@ -1875,215 +1896,221 @@
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="5"/>
+      <c r="L33" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="4"/>
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="8"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="7"/>
     </row>
     <row r="35" spans="4:15">
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="5"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="4"/>
     </row>
     <row r="36" spans="4:15">
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="7"/>
-      <c r="N36" s="7"/>
-      <c r="O36" s="8"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="7"/>
     </row>
     <row r="37" spans="4:15">
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="5"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="4"/>
     </row>
     <row r="38" spans="4:15">
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
-      <c r="O38" s="8"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="7"/>
     </row>
     <row r="39" spans="4:15">
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="5"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="4"/>
     </row>
     <row r="40" spans="4:15">
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
-      <c r="L40" s="6"/>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="8"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="7"/>
     </row>
     <row r="41" spans="4:15">
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="5"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="4"/>
     </row>
     <row r="42" spans="4:15">
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
-      <c r="L42" s="6"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="7"/>
-      <c r="O42" s="8"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="7"/>
     </row>
     <row r="43" spans="4:15">
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="5"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="4"/>
     </row>
     <row r="44" spans="4:15">
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
-      <c r="L44" s="6"/>
-      <c r="M44" s="7"/>
-      <c r="N44" s="7"/>
-      <c r="O44" s="8"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="6"/>
+      <c r="N44" s="6"/>
+      <c r="O44" s="7"/>
     </row>
     <row r="45" spans="4:15">
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-      <c r="O45" s="5"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="O45" s="4"/>
     </row>
     <row r="46" spans="4:15">
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
-      <c r="L46" s="6"/>
-      <c r="M46" s="7"/>
-      <c r="N46" s="7"/>
-      <c r="O46" s="8"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="6"/>
+      <c r="O46" s="7"/>
     </row>
     <row r="47" spans="4:7">
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
     </row>
     <row r="48" spans="4:7">
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="87">

</xml_diff>